<commit_message>
Modified format tables in: Ambits_sve,Ambits_rang,Ambits_Rang_SVE_mes,Ambits_verificació
</commit_message>
<xml_diff>
--- a/Metaarxius/taula3_historica.xlsx
+++ b/Metaarxius/taula3_historica.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="371">
   <si>
     <t>SVE</t>
   </si>
@@ -119,6 +119,12 @@
     <t>SE2_CNI</t>
   </si>
   <si>
+    <t>SE3_CI</t>
+  </si>
+  <si>
+    <t>SE3_CNI</t>
+  </si>
+  <si>
     <t>Barcelona Ciutat</t>
   </si>
   <si>
@@ -1059,6 +1065,66 @@
   </si>
   <si>
     <t>7597.0</t>
+  </si>
+  <si>
+    <t>2779.0</t>
+  </si>
+  <si>
+    <t>2921.0</t>
+  </si>
+  <si>
+    <t>3578.0</t>
+  </si>
+  <si>
+    <t>1326.0</t>
+  </si>
+  <si>
+    <t>1770.0</t>
+  </si>
+  <si>
+    <t>863.0</t>
+  </si>
+  <si>
+    <t>1375.0</t>
+  </si>
+  <si>
+    <t>511.0</t>
+  </si>
+  <si>
+    <t>797.0</t>
+  </si>
+  <si>
+    <t>15920.0</t>
+  </si>
+  <si>
+    <t>3381.0</t>
+  </si>
+  <si>
+    <t>2865.0</t>
+  </si>
+  <si>
+    <t>2746.0</t>
+  </si>
+  <si>
+    <t>779.0</t>
+  </si>
+  <si>
+    <t>736.0</t>
+  </si>
+  <si>
+    <t>562.0</t>
+  </si>
+  <si>
+    <t>1021.0</t>
+  </si>
+  <si>
+    <t>435.0</t>
+  </si>
+  <si>
+    <t>729.0</t>
+  </si>
+  <si>
+    <t>13254.0</t>
   </si>
 </sst>
 </file>
@@ -1215,1075 +1281,1141 @@
       <c r="AI1" t="s">
         <v>34</v>
       </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="D2" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="I2" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="J2" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="K2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="L2" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="M2" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="N2" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="O2" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="P2" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="Q2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="R2" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="S2" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="T2" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="U2" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="V2" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="W2" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="X2" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="Y2" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="Z2" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="AA2" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="AB2" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AC2" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="AD2" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AE2" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AF2" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="AG2" t="s">
-        <v>339</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>2779.0</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>3381.0</v>
+        <v>341</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>351</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>361</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>2636.0</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>2586.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="E3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="F3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="G3" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="I3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="K3" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="L3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="M3" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="N3" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="O3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="P3" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="Q3" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="R3" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="S3" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="T3" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="U3" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="V3" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="W3" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="X3" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="Y3" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="Z3" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="AA3" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="AB3" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AC3" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AD3" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AE3" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AF3" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="AG3" t="s">
-        <v>340</v>
-      </c>
-      <c r="AH3" t="n">
-        <v>2921.0</v>
-      </c>
-      <c r="AI3" t="n">
-        <v>2865.0</v>
+        <v>342</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>352</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>362</v>
+      </c>
+      <c r="AJ3" t="n">
+        <v>2231.0</v>
+      </c>
+      <c r="AK3" t="n">
+        <v>1726.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D4" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I4" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J4" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K4" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="M4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="N4" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="O4" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="P4" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="Q4" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="R4" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="S4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="T4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="U4" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="V4" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="W4" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="X4" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="Y4" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="Z4" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AA4" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="AB4" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="AC4" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AD4" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="AE4" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AF4" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="AG4" t="s">
-        <v>341</v>
-      </c>
-      <c r="AH4" t="n">
-        <v>3578.0</v>
-      </c>
-      <c r="AI4" t="n">
-        <v>2746.0</v>
+        <v>343</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>353</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>363</v>
+      </c>
+      <c r="AJ4" t="n">
+        <v>2382.0</v>
+      </c>
+      <c r="AK4" t="n">
+        <v>2312.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s">
+        <v>88</v>
+      </c>
+      <c r="G5" t="s">
+        <v>98</v>
+      </c>
+      <c r="H5" t="s">
+        <v>108</v>
+      </c>
+      <c r="I5" t="s">
         <v>58</v>
       </c>
-      <c r="D5" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F5" t="s">
-        <v>86</v>
-      </c>
-      <c r="G5" t="s">
-        <v>96</v>
-      </c>
-      <c r="H5" t="s">
-        <v>106</v>
-      </c>
-      <c r="I5" t="s">
-        <v>56</v>
-      </c>
       <c r="J5" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K5" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L5" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="M5" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N5" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="O5" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="P5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="Q5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="R5" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="S5" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="T5" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="U5" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="V5" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="W5" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="X5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="Y5" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="Z5" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AA5" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="AB5" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="AC5" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="AD5" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="AE5" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AF5" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="AG5" t="s">
-        <v>342</v>
-      </c>
-      <c r="AH5" t="n">
-        <v>1326.0</v>
-      </c>
-      <c r="AI5" t="n">
-        <v>779.0</v>
+        <v>344</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>354</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>364</v>
+      </c>
+      <c r="AJ5" t="n">
+        <v>841.0</v>
+      </c>
+      <c r="AK5" t="n">
+        <v>404.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D6" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="F6" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H6" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I6" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="K6" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L6" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="M6" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="N6" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="O6" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="P6" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="Q6" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="R6" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="S6" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="T6" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="U6" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="V6" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="W6" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="X6" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="Y6" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Z6" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="AA6" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AB6" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AC6" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="AD6" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="AE6" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AF6" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="AG6" t="s">
-        <v>343</v>
-      </c>
-      <c r="AH6" t="n">
-        <v>1770.0</v>
-      </c>
-      <c r="AI6" t="n">
-        <v>736.0</v>
+        <v>345</v>
+      </c>
+      <c r="AH6" t="s">
+        <v>355</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>365</v>
+      </c>
+      <c r="AJ6" t="n">
+        <v>1322.0</v>
+      </c>
+      <c r="AK6" t="n">
+        <v>652.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D7" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E7" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F7" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="G7" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="I7" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J7" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K7" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L7" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M7" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N7" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="O7" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="P7" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Q7" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="R7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="S7" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="T7" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="U7" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="V7" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="W7" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="X7" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="Y7" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="Z7" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="AA7" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AB7" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="AC7" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="AD7" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AE7" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="AF7" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AG7" t="s">
-        <v>344</v>
-      </c>
-      <c r="AH7" t="n">
-        <v>863.0</v>
-      </c>
-      <c r="AI7" t="n">
-        <v>562.0</v>
+        <v>346</v>
+      </c>
+      <c r="AH7" t="s">
+        <v>356</v>
+      </c>
+      <c r="AI7" t="s">
+        <v>366</v>
+      </c>
+      <c r="AJ7" t="n">
+        <v>538.0</v>
+      </c>
+      <c r="AK7" t="n">
+        <v>434.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F8" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G8" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H8" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I8" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J8" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="L8" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="M8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="N8" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="O8" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="P8" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Q8" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="R8" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="S8" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="T8" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="U8" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="V8" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="W8" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="X8" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="Y8" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="Z8" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="AA8" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AB8" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AC8" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="AD8" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="AE8" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AF8" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AG8" t="s">
-        <v>345</v>
-      </c>
-      <c r="AH8" t="n">
-        <v>1375.0</v>
-      </c>
-      <c r="AI8" t="n">
-        <v>1021.0</v>
+        <v>347</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>357</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>367</v>
+      </c>
+      <c r="AJ8" t="n">
+        <v>1100.0</v>
+      </c>
+      <c r="AK8" t="n">
+        <v>679.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E9" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G9" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H9" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I9" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J9" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K9" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L9" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="M9" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N9" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="O9" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="P9" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q9" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="R9" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="S9" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="T9" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="U9" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="V9" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="W9" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="X9" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="Y9" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="Z9" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AA9" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="AB9" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="AC9" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AD9" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AE9" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF9" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AG9" t="s">
-        <v>346</v>
-      </c>
-      <c r="AH9" t="n">
-        <v>511.0</v>
-      </c>
-      <c r="AI9" t="n">
-        <v>435.0</v>
+        <v>348</v>
+      </c>
+      <c r="AH9" t="s">
+        <v>358</v>
+      </c>
+      <c r="AI9" t="s">
+        <v>368</v>
+      </c>
+      <c r="AJ9" t="n">
+        <v>432.0</v>
+      </c>
+      <c r="AK9" t="n">
+        <v>287.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E10" t="s">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s">
+        <v>93</v>
+      </c>
+      <c r="G10" t="s">
+        <v>103</v>
+      </c>
+      <c r="H10" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" t="s">
+        <v>132</v>
+      </c>
+      <c r="K10" t="s">
+        <v>141</v>
+      </c>
+      <c r="L10" t="s">
+        <v>151</v>
+      </c>
+      <c r="M10" t="s">
+        <v>161</v>
+      </c>
+      <c r="N10" t="s">
+        <v>171</v>
+      </c>
+      <c r="O10" t="s">
+        <v>181</v>
+      </c>
+      <c r="P10" t="s">
+        <v>190</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>199</v>
+      </c>
+      <c r="R10" t="s">
+        <v>207</v>
+      </c>
+      <c r="S10" t="s">
+        <v>217</v>
+      </c>
+      <c r="T10" t="s">
+        <v>226</v>
+      </c>
+      <c r="U10" t="s">
+        <v>236</v>
+      </c>
+      <c r="V10" t="s">
+        <v>246</v>
+      </c>
+      <c r="W10" t="s">
+        <v>140</v>
+      </c>
+      <c r="X10" t="s">
         <v>73</v>
       </c>
-      <c r="E10" t="s">
+      <c r="Y10" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>281</v>
+      </c>
+      <c r="AA10" t="s">
         <v>81</v>
       </c>
-      <c r="F10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G10" t="s">
-        <v>101</v>
-      </c>
-      <c r="H10" t="s">
-        <v>111</v>
-      </c>
-      <c r="I10" t="s">
-        <v>120</v>
-      </c>
-      <c r="J10" t="s">
-        <v>130</v>
-      </c>
-      <c r="K10" t="s">
-        <v>139</v>
-      </c>
-      <c r="L10" t="s">
-        <v>149</v>
-      </c>
-      <c r="M10" t="s">
-        <v>159</v>
-      </c>
-      <c r="N10" t="s">
-        <v>169</v>
-      </c>
-      <c r="O10" t="s">
-        <v>179</v>
-      </c>
-      <c r="P10" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>197</v>
-      </c>
-      <c r="R10" t="s">
-        <v>205</v>
-      </c>
-      <c r="S10" t="s">
-        <v>215</v>
-      </c>
-      <c r="T10" t="s">
-        <v>224</v>
-      </c>
-      <c r="U10" t="s">
-        <v>234</v>
-      </c>
-      <c r="V10" t="s">
-        <v>244</v>
-      </c>
-      <c r="W10" t="s">
-        <v>138</v>
-      </c>
-      <c r="X10" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>270</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>279</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>79</v>
-      </c>
       <c r="AB10" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="AC10" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AD10" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AE10" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AF10" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AG10" t="s">
-        <v>347</v>
-      </c>
-      <c r="AH10" t="n">
-        <v>797.0</v>
-      </c>
-      <c r="AI10" t="n">
-        <v>729.0</v>
+        <v>349</v>
+      </c>
+      <c r="AH10" t="s">
+        <v>359</v>
+      </c>
+      <c r="AI10" t="s">
+        <v>369</v>
+      </c>
+      <c r="AJ10" t="n">
+        <v>522.0</v>
+      </c>
+      <c r="AK10" t="n">
+        <v>537.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D11" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E11" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F11" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G11" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H11" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I11" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J11" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K11" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L11" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="M11" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="N11" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="O11" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="P11" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="Q11" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="R11" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="S11" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="T11" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="U11" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="V11" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="W11" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="X11" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="Y11" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="Z11" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AA11" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="AB11" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="AC11" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AD11" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AE11" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AF11" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="AG11" t="s">
-        <v>348</v>
-      </c>
-      <c r="AH11" t="n">
-        <v>15920.0</v>
-      </c>
-      <c r="AI11" t="n">
-        <v>13254.0</v>
+        <v>350</v>
+      </c>
+      <c r="AH11" t="s">
+        <v>360</v>
+      </c>
+      <c r="AI11" t="s">
+        <v>370</v>
+      </c>
+      <c r="AJ11" t="n">
+        <v>12004.0</v>
+      </c>
+      <c r="AK11" t="n">
+        <v>9617.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified taula 8 without escolars. Modified fig 1 and 2 substracting escolars. Deletes tables 8a and b
</commit_message>
<xml_diff>
--- a/Metaarxius/taula3_historica.xlsx
+++ b/Metaarxius/taula3_historica.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="393">
   <si>
     <t>SVE</t>
   </si>
@@ -125,6 +125,12 @@
     <t>SE3_CNI</t>
   </si>
   <si>
+    <t>SE4_CI</t>
+  </si>
+  <si>
+    <t>SE4_CNI</t>
+  </si>
+  <si>
     <t>Barcelona Ciutat</t>
   </si>
   <si>
@@ -1125,6 +1131,66 @@
   </si>
   <si>
     <t>13254.0</t>
+  </si>
+  <si>
+    <t>2636.0</t>
+  </si>
+  <si>
+    <t>2231.0</t>
+  </si>
+  <si>
+    <t>2382.0</t>
+  </si>
+  <si>
+    <t>841.0</t>
+  </si>
+  <si>
+    <t>1322.0</t>
+  </si>
+  <si>
+    <t>538.0</t>
+  </si>
+  <si>
+    <t>1100.0</t>
+  </si>
+  <si>
+    <t>432.0</t>
+  </si>
+  <si>
+    <t>522.0</t>
+  </si>
+  <si>
+    <t>12004.0</t>
+  </si>
+  <si>
+    <t>2586.0</t>
+  </si>
+  <si>
+    <t>1726.0</t>
+  </si>
+  <si>
+    <t>2312.0</t>
+  </si>
+  <si>
+    <t>404.0</t>
+  </si>
+  <si>
+    <t>652.0</t>
+  </si>
+  <si>
+    <t>434.0</t>
+  </si>
+  <si>
+    <t>679.0</t>
+  </si>
+  <si>
+    <t>287.0</t>
+  </si>
+  <si>
+    <t>537.0</t>
+  </si>
+  <si>
+    <t>9617.0</t>
   </si>
 </sst>
 </file>
@@ -1287,1135 +1353,1201 @@
       <c r="AK1" t="s">
         <v>36</v>
       </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="E2" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="I2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J2" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="L2" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="M2" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="N2" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="O2" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="P2" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="Q2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="R2" t="s">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="S2" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="T2" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="U2" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="V2" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="W2" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="X2" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="Y2" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="Z2" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="AA2" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="AB2" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="AC2" t="s">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="AD2" t="s">
-        <v>311</v>
+        <v>313</v>
       </c>
       <c r="AE2" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="AF2" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="AG2" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="AH2" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="AI2" t="s">
-        <v>361</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>2636.0</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>2586.0</v>
+        <v>363</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>373</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>383</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>2442.0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>2205.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="G3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="I3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J3" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="K3" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="L3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="M3" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="N3" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="O3" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="P3" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="Q3" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="R3" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="S3" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="T3" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="U3" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="V3" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="W3" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="X3" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="Y3" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="Z3" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="AA3" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="AB3" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="AC3" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="AD3" t="s">
-        <v>312</v>
+        <v>314</v>
       </c>
       <c r="AE3" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="AF3" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="AG3" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="AH3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="AI3" t="s">
-        <v>362</v>
-      </c>
-      <c r="AJ3" t="n">
-        <v>2231.0</v>
-      </c>
-      <c r="AK3" t="n">
-        <v>1726.0</v>
+        <v>364</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>374</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>384</v>
+      </c>
+      <c r="AL3" t="n">
+        <v>2250.0</v>
+      </c>
+      <c r="AM3" t="n">
+        <v>1586.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C4" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="F4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H4" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="I4" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J4" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="K4" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="L4" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="M4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="N4" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="O4" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="P4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="Q4" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="R4" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="S4" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="T4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="U4" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="V4" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="W4" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="X4" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="Y4" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="Z4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="AA4" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="AB4" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="AC4" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="AD4" t="s">
-        <v>313</v>
+        <v>315</v>
       </c>
       <c r="AE4" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="AF4" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="AG4" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="AH4" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="AI4" t="s">
-        <v>363</v>
-      </c>
-      <c r="AJ4" t="n">
-        <v>2382.0</v>
-      </c>
-      <c r="AK4" t="n">
-        <v>2312.0</v>
+        <v>365</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>375</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>385</v>
+      </c>
+      <c r="AL4" t="n">
+        <v>2258.0</v>
+      </c>
+      <c r="AM4" t="n">
+        <v>1632.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D5" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H5" t="s">
+        <v>110</v>
+      </c>
+      <c r="I5" t="s">
         <v>60</v>
       </c>
-      <c r="D5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F5" t="s">
-        <v>88</v>
-      </c>
-      <c r="G5" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I5" t="s">
-        <v>58</v>
-      </c>
       <c r="J5" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K5" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="L5" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="M5" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="N5" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="O5" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="P5" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="Q5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="R5" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="S5" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="T5" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="U5" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="V5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="W5" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="X5" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="Y5" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="Z5" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="AA5" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="AB5" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="AC5" t="s">
-        <v>304</v>
+        <v>306</v>
       </c>
       <c r="AD5" t="s">
-        <v>314</v>
+        <v>316</v>
       </c>
       <c r="AE5" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="AF5" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="AG5" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="AH5" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="AI5" t="s">
-        <v>364</v>
-      </c>
-      <c r="AJ5" t="n">
-        <v>841.0</v>
-      </c>
-      <c r="AK5" t="n">
-        <v>404.0</v>
+        <v>366</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>376</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>386</v>
+      </c>
+      <c r="AL5" t="n">
+        <v>852.0</v>
+      </c>
+      <c r="AM5" t="n">
+        <v>372.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E6" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="G6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H6" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="I6" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J6" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="K6" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="L6" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="M6" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="N6" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="O6" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="P6" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="Q6" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="R6" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="S6" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="T6" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="U6" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="V6" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="W6" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="X6" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="Y6" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="Z6" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="AA6" t="s">
-        <v>287</v>
+        <v>289</v>
       </c>
       <c r="AB6" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="AC6" t="s">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="AD6" t="s">
-        <v>315</v>
+        <v>317</v>
       </c>
       <c r="AE6" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="AF6" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="AG6" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="AH6" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="AI6" t="s">
-        <v>365</v>
-      </c>
-      <c r="AJ6" t="n">
-        <v>1322.0</v>
-      </c>
-      <c r="AK6" t="n">
-        <v>652.0</v>
+        <v>367</v>
+      </c>
+      <c r="AJ6" t="s">
+        <v>377</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>387</v>
+      </c>
+      <c r="AL6" t="n">
+        <v>1371.0</v>
+      </c>
+      <c r="AM6" t="n">
+        <v>589.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="E7" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G7" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H7" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="I7" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="J7" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="K7" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="L7" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="M7" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="N7" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="O7" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="P7" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="Q7" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="R7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="S7" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="T7" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="U7" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="V7" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="W7" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="X7" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="Y7" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="Z7" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="AA7" t="s">
-        <v>288</v>
+        <v>290</v>
       </c>
       <c r="AB7" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="AC7" t="s">
-        <v>306</v>
+        <v>308</v>
       </c>
       <c r="AD7" t="s">
-        <v>316</v>
+        <v>318</v>
       </c>
       <c r="AE7" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="AF7" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="AG7" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
       <c r="AH7" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="AI7" t="s">
-        <v>366</v>
-      </c>
-      <c r="AJ7" t="n">
-        <v>538.0</v>
-      </c>
-      <c r="AK7" t="n">
-        <v>434.0</v>
+        <v>368</v>
+      </c>
+      <c r="AJ7" t="s">
+        <v>378</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>388</v>
+      </c>
+      <c r="AL7" t="n">
+        <v>722.0</v>
+      </c>
+      <c r="AM7" t="n">
+        <v>616.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="D8" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H8" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="I8" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J8" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="K8" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="L8" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="M8" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="N8" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="O8" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="P8" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="Q8" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="R8" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="S8" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="T8" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="U8" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="V8" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="W8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="X8" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="Y8" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="Z8" t="s">
-        <v>279</v>
+        <v>281</v>
       </c>
       <c r="AA8" t="s">
-        <v>289</v>
+        <v>291</v>
       </c>
       <c r="AB8" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="AC8" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="AD8" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="AE8" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="AF8" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="AG8" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="AH8" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="AI8" t="s">
-        <v>367</v>
-      </c>
-      <c r="AJ8" t="n">
-        <v>1100.0</v>
-      </c>
-      <c r="AK8" t="n">
-        <v>679.0</v>
+        <v>369</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>379</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>389</v>
+      </c>
+      <c r="AL8" t="n">
+        <v>947.0</v>
+      </c>
+      <c r="AM8" t="n">
+        <v>583.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B9" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C9" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D9" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="E9" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="F9" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="G9" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="I9" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="J9" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="K9" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="L9" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="M9" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="N9" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="O9" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="P9" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="Q9" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="R9" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="S9" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="T9" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="U9" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="V9" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="W9" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="X9" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="Y9" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="Z9" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
       <c r="AA9" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="AB9" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="AC9" t="s">
-        <v>308</v>
+        <v>310</v>
       </c>
       <c r="AD9" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="AE9" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="AF9" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="AG9" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="AH9" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="AI9" t="s">
-        <v>368</v>
-      </c>
-      <c r="AJ9" t="n">
-        <v>432.0</v>
-      </c>
-      <c r="AK9" t="n">
-        <v>287.0</v>
+        <v>370</v>
+      </c>
+      <c r="AJ9" t="s">
+        <v>380</v>
+      </c>
+      <c r="AK9" t="s">
+        <v>390</v>
+      </c>
+      <c r="AL9" t="n">
+        <v>558.0</v>
+      </c>
+      <c r="AM9" t="n">
+        <v>137.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="E10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F10" t="s">
+        <v>95</v>
+      </c>
+      <c r="G10" t="s">
+        <v>105</v>
+      </c>
+      <c r="H10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I10" t="s">
+        <v>124</v>
+      </c>
+      <c r="J10" t="s">
+        <v>134</v>
+      </c>
+      <c r="K10" t="s">
+        <v>143</v>
+      </c>
+      <c r="L10" t="s">
+        <v>153</v>
+      </c>
+      <c r="M10" t="s">
+        <v>163</v>
+      </c>
+      <c r="N10" t="s">
+        <v>173</v>
+      </c>
+      <c r="O10" t="s">
+        <v>183</v>
+      </c>
+      <c r="P10" t="s">
+        <v>192</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>201</v>
+      </c>
+      <c r="R10" t="s">
+        <v>209</v>
+      </c>
+      <c r="S10" t="s">
+        <v>219</v>
+      </c>
+      <c r="T10" t="s">
+        <v>228</v>
+      </c>
+      <c r="U10" t="s">
+        <v>238</v>
+      </c>
+      <c r="V10" t="s">
+        <v>248</v>
+      </c>
+      <c r="W10" t="s">
+        <v>142</v>
+      </c>
+      <c r="X10" t="s">
         <v>75</v>
       </c>
-      <c r="E10" t="s">
+      <c r="Y10" t="s">
+        <v>274</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>283</v>
+      </c>
+      <c r="AA10" t="s">
         <v>83</v>
       </c>
-      <c r="F10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G10" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" t="s">
-        <v>113</v>
-      </c>
-      <c r="I10" t="s">
-        <v>122</v>
-      </c>
-      <c r="J10" t="s">
-        <v>132</v>
-      </c>
-      <c r="K10" t="s">
-        <v>141</v>
-      </c>
-      <c r="L10" t="s">
-        <v>151</v>
-      </c>
-      <c r="M10" t="s">
-        <v>161</v>
-      </c>
-      <c r="N10" t="s">
-        <v>171</v>
-      </c>
-      <c r="O10" t="s">
-        <v>181</v>
-      </c>
-      <c r="P10" t="s">
-        <v>190</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>199</v>
-      </c>
-      <c r="R10" t="s">
-        <v>207</v>
-      </c>
-      <c r="S10" t="s">
-        <v>217</v>
-      </c>
-      <c r="T10" t="s">
-        <v>226</v>
-      </c>
-      <c r="U10" t="s">
-        <v>236</v>
-      </c>
-      <c r="V10" t="s">
-        <v>246</v>
-      </c>
-      <c r="W10" t="s">
-        <v>140</v>
-      </c>
-      <c r="X10" t="s">
-        <v>73</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>272</v>
-      </c>
-      <c r="Z10" t="s">
-        <v>281</v>
-      </c>
-      <c r="AA10" t="s">
-        <v>81</v>
-      </c>
       <c r="AB10" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="AC10" t="s">
-        <v>309</v>
+        <v>311</v>
       </c>
       <c r="AD10" t="s">
-        <v>319</v>
+        <v>321</v>
       </c>
       <c r="AE10" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="AF10" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="AG10" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="AH10" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="AI10" t="s">
-        <v>369</v>
-      </c>
-      <c r="AJ10" t="n">
-        <v>522.0</v>
-      </c>
-      <c r="AK10" t="n">
-        <v>537.0</v>
+        <v>371</v>
+      </c>
+      <c r="AJ10" t="s">
+        <v>381</v>
+      </c>
+      <c r="AK10" t="s">
+        <v>391</v>
+      </c>
+      <c r="AL10" t="n">
+        <v>835.0</v>
+      </c>
+      <c r="AM10" t="n">
+        <v>584.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="F11" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="G11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H11" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="I11" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K11" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="L11" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="M11" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="N11" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="O11" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="P11" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="Q11" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="R11" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="S11" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="T11" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="U11" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="V11" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="W11" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="X11" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="Y11" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="Z11" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="AA11" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="AB11" t="s">
-        <v>300</v>
+        <v>302</v>
       </c>
       <c r="AC11" t="s">
-        <v>310</v>
+        <v>312</v>
       </c>
       <c r="AD11" t="s">
-        <v>320</v>
+        <v>322</v>
       </c>
       <c r="AE11" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="AF11" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="AG11" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="AH11" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="AI11" t="s">
-        <v>370</v>
-      </c>
-      <c r="AJ11" t="n">
-        <v>12004.0</v>
-      </c>
-      <c r="AK11" t="n">
-        <v>9617.0</v>
+        <v>372</v>
+      </c>
+      <c r="AJ11" t="s">
+        <v>382</v>
+      </c>
+      <c r="AK11" t="s">
+        <v>392</v>
+      </c>
+      <c r="AL11" t="n">
+        <v>12235.0</v>
+      </c>
+      <c r="AM11" t="n">
+        <v>8304.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>